<commit_message>
Checked first part of pre-run check list
</commit_message>
<xml_diff>
--- a/repswitch_V1L1.xlsx
+++ b/repswitch_V1L1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B3AD3D-4BBA-4324-B78D-01B372B55700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4A3549-4898-4552-A39F-3871CC59B2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="600" windowWidth="10596" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="11" r:id="rId1"/>
@@ -1379,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BB0F28-4100-4959-A1B4-04A785FFC3D9}">
   <dimension ref="A1:S409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changed column name from "trial" to "trial_no"
Received warning from PsychoPy that variable "trial" was used two times.
</commit_message>
<xml_diff>
--- a/repswitch_V1L1.xlsx
+++ b/repswitch_V1L1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4A3549-4898-4552-A39F-3871CC59B2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2294C88-AD5B-4AB2-84C2-B80AD45D615A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="600" windowWidth="10596" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="11" r:id="rId1"/>
@@ -395,9 +395,6 @@
     <t>columna</t>
   </si>
   <si>
-    <t>trial</t>
-  </si>
-  <si>
     <t>psychopy_trial</t>
   </si>
   <si>
@@ -462,6 +459,9 @@
   </si>
   <si>
     <t>REPSWITCH1/PICTURE_381.png</t>
+  </si>
+  <si>
+    <t>trial_no</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1082,7 @@
     <tableColumn id="9" xr3:uid="{D8BE28D8-E777-4FE4-93DB-026714227EA3}" name="stimulus" dataDxfId="5"/>
     <tableColumn id="10" xr3:uid="{6987E22D-5B0B-4D47-AF0A-CEB0F46E83C0}" name="baseline" dataDxfId="4"/>
     <tableColumn id="11" xr3:uid="{E76A761E-3112-4230-B2DD-7421C9606EEF}" name="baseline_condition" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{8D935A5E-FBA8-4E96-B510-722A9BE4CB44}" name="trial" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{8D935A5E-FBA8-4E96-B510-722A9BE4CB44}" name="trial_no" dataDxfId="2"/>
     <tableColumn id="13" xr3:uid="{6A72032C-08C8-4CBB-8C23-6471D214F180}" name="psychopy_trial" dataDxfId="1"/>
     <tableColumn id="16" xr3:uid="{9031910A-C319-4A14-9ECB-83FC68DEF03C}" name="Column1" dataDxfId="0"/>
   </tableColumns>
@@ -1380,7 +1380,7 @@
   <dimension ref="A1:S409"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1415,36 +1415,36 @@
         <v>40</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="O1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>121</v>
-      </c>
       <c r="Q1" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>114</v>
@@ -1477,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M2" s="10">
         <v>0</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>115</v>
@@ -1528,7 +1528,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M3" s="7">
         <v>0</v>
@@ -1701,10 +1701,10 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>4</v>
@@ -1754,10 +1754,10 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -2062,7 +2062,7 @@
         <v>12</v>
       </c>
       <c r="S13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -2946,10 +2946,10 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>4</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>116</v>
@@ -3909,7 +3909,7 @@
         <v>1</v>
       </c>
       <c r="L49" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M49" s="7">
         <v>0</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B55" s="16" t="s">
         <v>117</v>
@@ -4217,7 +4217,7 @@
         <v>1</v>
       </c>
       <c r="L55" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M55" s="7">
         <v>0</v>
@@ -4910,7 +4910,7 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>118</v>
@@ -4943,7 +4943,7 @@
         <v>1</v>
       </c>
       <c r="L69" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M69" s="7">
         <v>0</v>
@@ -6303,7 +6303,7 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B96" s="16" t="s">
         <v>119</v>
@@ -6336,7 +6336,7 @@
         <v>1</v>
       </c>
       <c r="L96" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M96" s="7">
         <v>0</v>
@@ -6711,7 +6711,7 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B104" s="16" t="s">
         <v>119</v>
@@ -6744,7 +6744,7 @@
         <v>1</v>
       </c>
       <c r="L104" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M104" s="10">
         <v>0</v>
@@ -7021,7 +7021,7 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B110" s="16" t="s">
         <v>118</v>
@@ -7054,7 +7054,7 @@
         <v>1</v>
       </c>
       <c r="L110" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M110" s="7">
         <v>0</v>
@@ -7280,10 +7280,10 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>5</v>
@@ -7333,10 +7333,10 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>4</v>
@@ -8726,10 +8726,10 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>4</v>
@@ -9291,7 +9291,7 @@
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B154" s="19" t="s">
         <v>116</v>
@@ -9324,7 +9324,7 @@
         <v>1</v>
       </c>
       <c r="L154" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M154" s="20">
         <v>0</v>
@@ -9652,7 +9652,7 @@
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B161" s="16" t="s">
         <v>115</v>
@@ -9685,7 +9685,7 @@
         <v>1</v>
       </c>
       <c r="L161" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M161" s="7">
         <v>0</v>
@@ -10319,7 +10319,7 @@
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B174" s="16" t="s">
         <v>117</v>
@@ -10352,7 +10352,7 @@
         <v>1</v>
       </c>
       <c r="L174" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M174" s="7">
         <v>0</v>
@@ -11869,7 +11869,7 @@
     </row>
     <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B204" s="16" t="s">
         <v>114</v>
@@ -11902,7 +11902,7 @@
         <v>1</v>
       </c>
       <c r="L204" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M204" s="7">
         <v>0</v>
@@ -11971,7 +11971,7 @@
     </row>
     <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B206" s="16" t="s">
         <v>117</v>
@@ -12004,7 +12004,7 @@
         <v>1</v>
       </c>
       <c r="L206" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M206" s="10">
         <v>0</v>
@@ -12022,7 +12022,7 @@
     </row>
     <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B207" s="16" t="s">
         <v>114</v>
@@ -12055,7 +12055,7 @@
         <v>1</v>
       </c>
       <c r="L207" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M207" s="10">
         <v>0</v>
@@ -12899,10 +12899,10 @@
     </row>
     <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C224" s="7" t="s">
         <v>5</v>
@@ -12952,10 +12952,10 @@
     </row>
     <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C225" s="7" t="s">
         <v>5</v>
@@ -14190,10 +14190,10 @@
     </row>
     <row r="249" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A249" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C249" s="7" t="s">
         <v>5</v>
@@ -16823,7 +16823,7 @@
     </row>
     <row r="300" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A300" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B300" s="16" t="s">
         <v>118</v>
@@ -16856,7 +16856,7 @@
         <v>1</v>
       </c>
       <c r="L300" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M300" s="7">
         <v>0</v>
@@ -16927,7 +16927,7 @@
     </row>
     <row r="302" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A302" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B302" s="16" t="s">
         <v>119</v>
@@ -16960,7 +16960,7 @@
         <v>1</v>
       </c>
       <c r="L302" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M302" s="7">
         <v>0</v>
@@ -17135,7 +17135,7 @@
     </row>
     <row r="306" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A306" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B306" s="16" t="s">
         <v>115</v>
@@ -17168,7 +17168,7 @@
         <v>1</v>
       </c>
       <c r="L306" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M306" s="7">
         <v>0</v>
@@ -17186,7 +17186,7 @@
     </row>
     <row r="307" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A307" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B307" s="19" t="s">
         <v>116</v>
@@ -17219,7 +17219,7 @@
         <v>1</v>
       </c>
       <c r="L307" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M307" s="20">
         <v>0</v>
@@ -17912,10 +17912,10 @@
     </row>
     <row r="321" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A321" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C321" s="7" t="s">
         <v>4</v>
@@ -17965,10 +17965,10 @@
     </row>
     <row r="322" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A322" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C322" s="7" t="s">
         <v>5</v>
@@ -18844,7 +18844,7 @@
     </row>
     <row r="339" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A339" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B339" s="16" t="s">
         <v>118</v>
@@ -18877,7 +18877,7 @@
         <v>1</v>
       </c>
       <c r="L339" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M339" s="7">
         <v>0</v>
@@ -19207,10 +19207,10 @@
     </row>
     <row r="346" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A346" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C346" s="7" t="s">
         <v>5</v>
@@ -19619,7 +19619,7 @@
     </row>
     <row r="354" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A354" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B354" s="16" t="s">
         <v>117</v>
@@ -19652,7 +19652,7 @@
         <v>1</v>
       </c>
       <c r="L354" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M354" s="7">
         <v>0</v>
@@ -19825,7 +19825,7 @@
     </row>
     <row r="358" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A358" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B358" s="19" t="s">
         <v>119</v>
@@ -19858,7 +19858,7 @@
         <v>1</v>
       </c>
       <c r="L358" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M358" s="3">
         <v>0</v>
@@ -21169,7 +21169,7 @@
     </row>
     <row r="384" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A384" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B384" s="16" t="s">
         <v>114</v>
@@ -21202,7 +21202,7 @@
         <v>1</v>
       </c>
       <c r="L384" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M384" s="7">
         <v>0</v>
@@ -21891,7 +21891,7 @@
     </row>
     <row r="398" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A398" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B398" s="16" t="s">
         <v>115</v>
@@ -21924,7 +21924,7 @@
         <v>1</v>
       </c>
       <c r="L398" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M398" s="7">
         <v>0</v>
@@ -22305,7 +22305,7 @@
     </row>
     <row r="406" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A406" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B406" s="16" t="s">
         <v>116</v>
@@ -22338,7 +22338,7 @@
         <v>1</v>
       </c>
       <c r="L406" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M406" s="7">
         <v>0</v>

</xml_diff>